<commit_message>
Final version of the work
</commit_message>
<xml_diff>
--- a/TP4/Resultados_Novos.xlsx
+++ b/TP4/Resultados_Novos.xlsx
@@ -564,7 +564,7 @@
   <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3936,7 +3936,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>